<commit_message>
Final code for 2025 ShellEco Marathon competition
</commit_message>
<xml_diff>
--- a/batt.xlsx
+++ b/batt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfranca\Development\GitHub\EcoMaua_BLDC_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC211819-5D9D-4634-A996-65092458BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EB1217-EDE2-4476-96DB-C33323FE356B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{72FA9700-AD12-4748-8300-7B4BA09846F0}"/>
   </bookViews>
@@ -174,17 +174,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.4087814623080961E-2"/>
-                  <c:y val="-0.18680883639545057"/>
+                  <c:x val="-0.12406738327720535"/>
+                  <c:y val="5.9389303475550076E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="&quot;R$&quot;\ #,##0.0000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -558,6 +559,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -565,7 +567,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1514,18 +1515,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8B76D5-E5EE-47FC-BF2C-804A22F9DD8B}">
-  <dimension ref="C2:F14"/>
+  <dimension ref="C2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" s="2">
         <v>4.2</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>4.0999999999999996</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5" s="2">
         <v>4</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <v>3.9</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <v>3.85</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>3.8</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9" s="2">
         <v>3.75</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>3.7</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <v>3.6</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>3.5</v>
       </c>
@@ -1625,11 +1626,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <v>4.1500000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="1">
+        <f>-344.6374*C15^3+3947.7404*C15^2-14903.3718*C15+18587.9621</f>
+        <v>96.530039775007026</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>